<commit_message>
Server 2.0.0 and BX 2.1.0 release plan.
</commit_message>
<xml_diff>
--- a/documentation/versioning.xlsx
+++ b/documentation/versioning.xlsx
@@ -4,22 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="19155" windowHeight="12585"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="19155" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="libbitcoin" sheetId="1" r:id="rId1"/>
+    <sheet name="spesmilo" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$48</definedName>
-  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="90">
   <si>
     <t>libbitcoin</t>
   </si>
@@ -171,9 +167,6 @@
     <t>branch purpose</t>
   </si>
   <si>
-    <t>obelisk</t>
-  </si>
-  <si>
     <t>release: sx, obelisk</t>
   </si>
   <si>
@@ -232,6 +225,66 @@
   </si>
   <si>
     <t>client-v2.0.0</t>
+  </si>
+  <si>
+    <t>release: bx, server</t>
+  </si>
+  <si>
+    <t>2.8.0</t>
+  </si>
+  <si>
+    <t>v2.8.0</t>
+  </si>
+  <si>
+    <t>Required by blockchain v2.0.0 and client v2.1.0.</t>
+  </si>
+  <si>
+    <t>release: server</t>
+  </si>
+  <si>
+    <t>bc-v2.8.0</t>
+  </si>
+  <si>
+    <t>client-v2.1.0</t>
+  </si>
+  <si>
+    <t>bx-v2.1.0</t>
+  </si>
+  <si>
+    <t>blockchain-v2.0.0</t>
+  </si>
+  <si>
+    <t>node-v2.0.0</t>
+  </si>
+  <si>
+    <t>server-v2.0.0</t>
+  </si>
+  <si>
+    <t>2.1.0</t>
+  </si>
+  <si>
+    <t>v2.1.0</t>
+  </si>
+  <si>
+    <t>Corresponds to bx v2.1.0.</t>
+  </si>
+  <si>
+    <t>Upgrade for server stealth features.</t>
+  </si>
+  <si>
+    <t>Required by server v2.0.0.</t>
+  </si>
+  <si>
+    <t>Initial release of server, successor to obelisk.</t>
+  </si>
+  <si>
+    <t>spesmilo: obelisk</t>
+  </si>
+  <si>
+    <t>libbitcoin-consensus</t>
+  </si>
+  <si>
+    <t>Required by node v2.0.0.</t>
   </si>
 </sst>
 </file>
@@ -269,7 +322,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -288,6 +341,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -301,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -311,6 +376,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,19 +688,21 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="64.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="62.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -669,281 +744,302 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
+      <c r="D4" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>47</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="F6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G7" t="s">
-        <v>26</v>
+      <c r="G7" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="6" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="6" t="s">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D18" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E18" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C24" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E17" t="s">
+      <c r="F24" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E18" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" t="s">
-        <v>35</v>
-      </c>
-      <c r="G24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
-        <v>55</v>
-      </c>
-      <c r="E25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
-        <v>55</v>
-      </c>
-      <c r="E26" t="s">
-        <v>41</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" t="s">
-        <v>42</v>
+      <c r="F26" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -957,12 +1053,12 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -976,215 +1072,252 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
+      <c r="A31" s="8"/>
+      <c r="B31" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>59</v>
+        <v>8</v>
+      </c>
+      <c r="E32" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>62</v>
-      </c>
-      <c r="C33" s="6" t="s">
+      <c r="A33" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C34" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
+      <c r="D34" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>61</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
+        <v>35</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
         <v>54</v>
       </c>
-      <c r="D35" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>63</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D36" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>51</v>
-      </c>
-      <c r="C37" t="s">
-        <v>3</v>
-      </c>
-      <c r="D37" t="s">
-        <v>55</v>
+      <c r="E37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E38" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C40" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C43" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" t="s">
+        <v>45</v>
+      </c>
+      <c r="D45" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D39" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C46" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="8"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D48" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E39" t="s">
-        <v>41</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>68</v>
-      </c>
-      <c r="C41" t="s">
-        <v>64</v>
-      </c>
-      <c r="D41" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C42" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D42" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D43" t="s">
-        <v>55</v>
-      </c>
-      <c r="E43" t="s">
-        <v>12</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G43" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D44" t="s">
-        <v>55</v>
-      </c>
-      <c r="E44" t="s">
-        <v>41</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>68</v>
-      </c>
-      <c r="C46" t="s">
-        <v>64</v>
-      </c>
-      <c r="D46" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C47" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D47" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D48" t="s">
-        <v>10</v>
-      </c>
-      <c r="E48" t="s">
-        <v>65</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G48" t="s">
-        <v>66</v>
-      </c>
+      <c r="F48" s="11"/>
+    </row>
+    <row r="49" spans="6:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F49" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1194,24 +1327,243 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="64.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Move some non-template file locations, update version history.
</commit_message>
<xml_diff>
--- a/documentation/versioning.xlsx
+++ b/documentation/versioning.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="libbitcoin" sheetId="1" r:id="rId1"/>
     <sheet name="spesmilo" sheetId="2" r:id="rId2"/>
+    <sheet name="signatures" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="98">
   <si>
     <t>libbitcoin</t>
   </si>
@@ -236,9 +237,6 @@
     <t>v2.8.0</t>
   </si>
   <si>
-    <t>Required by blockchain v2.0.0 and client v2.1.0.</t>
-  </si>
-  <si>
     <t>release: server</t>
   </si>
   <si>
@@ -266,9 +264,6 @@
     <t>v2.1.0</t>
   </si>
   <si>
-    <t>Corresponds to bx v2.1.0.</t>
-  </si>
-  <si>
     <t>Required by server v2.0.0.</t>
   </si>
   <si>
@@ -306,6 +301,15 @@
   </si>
   <si>
     <t>Upgrade for server changes and bip39.</t>
+  </si>
+  <si>
+    <t>Required by bx v2.1.0 and server v2.0.0.</t>
+  </si>
+  <si>
+    <t>Required by bx v2.1.0.</t>
+  </si>
+  <si>
+    <t>v1.0.0</t>
   </si>
 </sst>
 </file>
@@ -754,8 +758,8 @@
   </sheetPr>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="M44" sqref="M44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,7 +833,7 @@
         <v>18</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -960,7 +964,7 @@
     <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>2</v>
@@ -975,7 +979,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -999,7 +1003,7 @@
         <v>37</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F17" s="15" t="s">
         <v>18</v>
@@ -1012,7 +1016,7 @@
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F18" s="15" t="s">
         <v>18</v>
@@ -1025,7 +1029,7 @@
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F19" s="15" t="s">
         <v>18</v>
@@ -1038,7 +1042,7 @@
       <c r="C20" s="11"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F20" s="15" t="s">
         <v>18</v>
@@ -1051,7 +1055,7 @@
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>18</v>
@@ -1064,7 +1068,7 @@
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F22" s="15" t="s">
         <v>18</v>
@@ -1103,7 +1107,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>87</v>
+        <v>34</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1113,91 +1117,93 @@
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="10"/>
+      <c r="D27" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="21" t="s">
-        <v>3</v>
+      <c r="B28" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>2</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E28" s="10"/>
-      <c r="F28" s="15"/>
+        <v>80</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>18</v>
+      </c>
       <c r="G28" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="3"/>
+      <c r="B29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>81</v>
-      </c>
+      <c r="A30" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
-      <c r="B31" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>2</v>
+      <c r="B31" s="10"/>
+      <c r="C31" s="11" t="s">
+        <v>1</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F31" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>83</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="E31" s="10"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="10"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>46</v>
-      </c>
-      <c r="C32" t="s">
-        <v>2</v>
-      </c>
-      <c r="D32" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" t="s">
-        <v>35</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="G32" t="s">
-        <v>36</v>
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F32" s="15"/>
+      <c r="G32" s="10" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1216,7 +1222,7 @@
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1226,16 +1232,16 @@
         <v>2</v>
       </c>
       <c r="D35" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E35" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="E35" s="10" t="s">
-        <v>82</v>
-      </c>
       <c r="F35" s="15" t="s">
         <v>18</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1305,7 +1311,7 @@
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>2</v>
@@ -1320,7 +1326,7 @@
         <v>18</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1388,7 +1394,7 @@
         <v>18</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1405,35 +1411,35 @@
     </row>
     <row r="50" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F50" s="16"/>
     </row>
     <row r="51" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F51" s="16"/>
     </row>
     <row r="52" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F52" s="16"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="65" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="64" orientation="landscape" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1458,7 +1464,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1678,4 +1684,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update for libbitcoin-consensus v1.2.0.
</commit_message>
<xml_diff>
--- a/documentation/versioning.xlsx
+++ b/documentation/versioning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="104">
   <si>
     <t>libbitcoin</t>
   </si>
@@ -309,16 +309,25 @@
     <t>v1.0.0</t>
   </si>
   <si>
-    <t>1.0.1</t>
-  </si>
-  <si>
-    <t>v1.0.1</t>
-  </si>
-  <si>
     <t>Corresponds to satoshi client v0.10.1.</t>
   </si>
   <si>
     <t>Upgrade for libbitcon server and bip39.</t>
+  </si>
+  <si>
+    <t>1.1.0</t>
+  </si>
+  <si>
+    <t>v1.1.0</t>
+  </si>
+  <si>
+    <t>v1.2.0</t>
+  </si>
+  <si>
+    <t>Corresponds to satoshi client v0.11.0.</t>
+  </si>
+  <si>
+    <t>1.2.0</t>
   </si>
 </sst>
 </file>
@@ -762,10 +771,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,7 +1166,7 @@
         <v>1</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="F31" s="13"/>
     </row>
@@ -1166,14 +1175,14 @@
         <v>3</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F32" s="13"/>
       <c r="G32" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1181,81 +1190,82 @@
         <v>3</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F33" s="13"/>
       <c r="G33" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F34" s="13"/>
+      <c r="G34" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="3"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C35" s="4" t="s">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="5" t="s">
+    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D37" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E37" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F36" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
+      <c r="F37" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
         <v>2</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>8</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E38" t="s">
         <v>35</v>
       </c>
-      <c r="F37" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G37" t="s">
+      <c r="F38" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
-        <v>54</v>
-      </c>
-      <c r="E38" t="s">
-        <v>12</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G38" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1263,157 +1273,171 @@
         <v>54</v>
       </c>
       <c r="E39" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="F39" s="12" t="s">
         <v>17</v>
       </c>
       <c r="G39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>54</v>
+      </c>
+      <c r="E40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="3"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C41" s="4" t="s">
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="3"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C42" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="5" t="s">
+    <row r="43" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C43" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D43" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E43" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F42" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G42" s="5" t="s">
+      <c r="F43" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G43" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="3"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C44" s="4" t="s">
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="3"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C45" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="3"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="3"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>48</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>45</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C47" s="4" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C48" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C48" s="5" t="s">
+    <row r="49" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C49" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D49" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="E49" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F48" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G48" s="5" t="s">
+      <c r="F49" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G49" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="5" t="s">
+    <row r="50" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D50" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F49" s="13"/>
-    </row>
-    <row r="50" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F50" s="13"/>
     </row>
-    <row r="51" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
+    <row r="51" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F51" s="13"/>
+    </row>
+    <row r="52" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="F51" s="13"/>
-    </row>
-    <row r="52" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="14" t="s">
+      <c r="F52" s="13"/>
+    </row>
+    <row r="53" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="F52" s="13"/>
-    </row>
-    <row r="53" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="15" t="s">
+      <c r="F53" s="13"/>
+    </row>
+    <row r="54" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="F53" s="13"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="16" t="s">
+      <c r="F54" s="13"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="16" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="17" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="17" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update tags for server stack 2.1.0 release.
</commit_message>
<xml_diff>
--- a/documentation/versioning.xlsx
+++ b/documentation/versioning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="111">
   <si>
     <t>libbitcoin</t>
   </si>
@@ -153,18 +153,12 @@
     <t>libbitcoin-protocol</t>
   </si>
   <si>
-    <t>protocol</t>
-  </si>
-  <si>
     <t>release: bx</t>
   </si>
   <si>
     <t>release: obelisk, sx</t>
   </si>
   <si>
-    <t>feature: protocol</t>
-  </si>
-  <si>
     <t>branch purpose</t>
   </si>
   <si>
@@ -192,9 +186,6 @@
     <t>now compatible with ZMQ 4.0 and many fixes for stability and uptime.</t>
   </si>
   <si>
-    <t>3.0.0</t>
-  </si>
-  <si>
     <t>libbitcoin-server</t>
   </si>
   <si>
@@ -328,6 +319,36 @@
   </si>
   <si>
     <t>1.2.0</t>
+  </si>
+  <si>
+    <t>2.9.0</t>
+  </si>
+  <si>
+    <t>v2.9.0</t>
+  </si>
+  <si>
+    <t>Required server v2.1.0.</t>
+  </si>
+  <si>
+    <t>Required by node v2.1.0.</t>
+  </si>
+  <si>
+    <t>bc-v2.9.0</t>
+  </si>
+  <si>
+    <t>blockchain-v2.1.0</t>
+  </si>
+  <si>
+    <t>node-v2.1.0</t>
+  </si>
+  <si>
+    <t>server-v2.1.0</t>
+  </si>
+  <si>
+    <t>Required by server v2.1.0.</t>
+  </si>
+  <si>
+    <t>Fix synchronization stall.</t>
   </si>
 </sst>
 </file>
@@ -445,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -467,6 +488,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,10 +797,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,7 +819,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
@@ -827,623 +853,761 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+      <c r="B4" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D4" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
+      <c r="D5" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="F7" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G8" t="s">
-        <v>26</v>
+      <c r="G8" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>17</v>
       </c>
       <c r="G12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="4" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
+      <c r="B16" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+      <c r="E17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19"/>
+    </row>
+    <row r="20" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="20"/>
+    </row>
+    <row r="21" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="20"/>
+    </row>
+    <row r="22" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="20"/>
+    </row>
+    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="20"/>
+    </row>
+    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="F26" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="9"/>
+      <c r="E27" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E28" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E29" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C30" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C34" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D35" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E36" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="5" t="s">
+      <c r="F36" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="3"/>
+    </row>
+    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F38" s="13"/>
+    </row>
+    <row r="39" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="20"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="F39" s="21"/>
+      <c r="G39" s="20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C40" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F40" s="13"/>
+      <c r="G40" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C41" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F41" s="13"/>
+      <c r="G41" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="3"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C43" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C44" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" t="s">
+        <v>35</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G45" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>52</v>
+      </c>
+      <c r="E46" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G46" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>52</v>
+      </c>
+      <c r="E47" t="s">
+        <v>41</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G47" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="3"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C49" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="20"/>
+      <c r="B50" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E50" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="F50" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50" s="20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F51" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="3"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C53" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="3"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C55" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="20"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D56" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E56" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="F56" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G56" s="20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C57" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F57" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F58" s="13"/>
+    </row>
+    <row r="59" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F59" s="13"/>
+    </row>
+    <row r="60" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E18" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E19" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="9"/>
-      <c r="E20" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E21" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E22" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" t="s">
-        <v>33</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E24" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E25" t="s">
-        <v>69</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F28" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D29" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" t="s">
-        <v>35</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G29" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="F60" s="13"/>
+    </row>
+    <row r="61" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F61" s="13"/>
+    </row>
+    <row r="62" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F62" s="13"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F31" s="13"/>
-    </row>
-    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="F32" s="13"/>
-      <c r="G32" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C33" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="F33" s="13"/>
-      <c r="G33" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F34" s="13"/>
-      <c r="G34" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="3"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C36" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D36" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F37" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>2</v>
-      </c>
-      <c r="D38" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" t="s">
-        <v>35</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G38" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D39" t="s">
-        <v>54</v>
-      </c>
-      <c r="E39" t="s">
-        <v>12</v>
-      </c>
-      <c r="F39" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G39" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D40" t="s">
-        <v>54</v>
-      </c>
-      <c r="E40" t="s">
-        <v>41</v>
-      </c>
-      <c r="F40" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G40" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="3"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C42" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D42" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F43" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="3"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C45" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D45" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="3"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>48</v>
-      </c>
-      <c r="C47" t="s">
-        <v>45</v>
-      </c>
-      <c r="D47" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C48" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D48" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C49" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F49" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G49" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F50" s="13"/>
-    </row>
-    <row r="51" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F51" s="13"/>
-    </row>
-    <row r="52" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="17" t="s">
         <v>89</v>
-      </c>
-      <c r="F52" s="13"/>
-    </row>
-    <row r="53" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="F53" s="13"/>
-    </row>
-    <row r="54" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="F54" s="13"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="17" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="63" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="54" orientation="landscape" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1468,7 +1632,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1480,13 +1644,13 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>53</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -1495,13 +1659,13 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -1510,13 +1674,13 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -1527,7 +1691,7 @@
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>12</v>
@@ -1536,7 +1700,7 @@
         <v>17</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1544,7 +1708,7 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>41</v>
@@ -1553,12 +1717,12 @@
         <v>17</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1570,13 +1734,13 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -1589,7 +1753,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -1600,7 +1764,7 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>12</v>
@@ -1617,7 +1781,7 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>41</v>
@@ -1631,7 +1795,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1643,13 +1807,13 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C13" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>66</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -1676,13 +1840,13 @@
         <v>10</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>17</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates for server stack 2.1.0 release.
</commit_message>
<xml_diff>
--- a/documentation/versioning.xlsx
+++ b/documentation/versioning.xlsx
@@ -348,7 +348,7 @@
     <t>Required by server v2.1.0.</t>
   </si>
   <si>
-    <t>Fix synchronization stall.</t>
+    <t>Fix synchronization stall, enhance config.</t>
   </si>
 </sst>
 </file>
@@ -800,7 +800,7 @@
   <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,7 +1034,7 @@
         <v>77</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="F16" s="21" t="s">
         <v>18</v>
@@ -1304,19 +1304,17 @@
       <c r="F38" s="13"/>
     </row>
     <row r="39" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="20"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="22" t="s">
+      <c r="C39" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D39" s="20" t="s">
+      <c r="D39" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="E39" s="20" t="s">
+      <c r="E39" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="F39" s="21"/>
-      <c r="G39" s="20" t="s">
+      <c r="F39" s="13"/>
+      <c r="G39" s="5" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tweak missing verison info.
</commit_message>
<xml_diff>
--- a/documentation/versioning.xlsx
+++ b/documentation/versioning.xlsx
@@ -799,8 +799,8 @@
   </sheetPr>
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>